<commit_message>
added an excel requirements traceability matrix that covers all test cases and associates them with one or more requirement
</commit_message>
<xml_diff>
--- a/RequirementsTraceabilityMatrixv2.xlsx
+++ b/RequirementsTraceabilityMatrixv2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5b8d95291df29679/Desktop/Jobs/Revature/Projects/AutomationProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blake\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{F0617567-C128-4FC1-B104-825C640EC451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB0F3CA4-CED5-45A8-AFD8-43BAC3A65067}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF44D7D1-EE1C-4F4A-8BCE-8CA24E97CBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{DCB976A7-4731-4573-8BFA-D471F91E56A7}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{DCB976A7-4731-4573-8BFA-D471F91E56A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>REQ-001</t>
   </si>
@@ -213,6 +213,63 @@
   </si>
   <si>
     <t>SCRUM-TC-152</t>
+  </si>
+  <si>
+    <t>As a User I want to Register an Account with the Planetarium so that I can Login Securely</t>
+  </si>
+  <si>
+    <t>As a User I want to add new planets to the Planetarium, so I can track the planet in the night sky</t>
+  </si>
+  <si>
+    <t> As a User I should not be able to add new planets to the Planetarium with incorrect credentials</t>
+  </si>
+  <si>
+    <t>As a User I want to Login to my Account so that I can Enter the Planetarium</t>
+  </si>
+  <si>
+    <t>As the System I don't want a user to Login to an Account using an invalid Username and Password combo so that I can ensure my user accounts are secure</t>
+  </si>
+  <si>
+    <t>As a User I want to Logout of my Account so that I can exit the Planetarium</t>
+  </si>
+  <si>
+    <t>As the System I don't want a user to bypass the Login page so that I can ensure the Planetarium is only for logged in users</t>
+  </si>
+  <si>
+    <t>As the System I don't want a user to Register an Account using invalid usernames and passwords so that I can ensure system requirements are met</t>
+  </si>
+  <si>
+    <t> As a User I should be able to add Moon (Positive Scenario)</t>
+  </si>
+  <si>
+    <t> As a User I should be able to add Moon (Negative Scenario)</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to remove Moons from the Planetarium</t>
+  </si>
+  <si>
+    <t>As a user I should not be able to remove Moon from the Planetarium when given invalid names</t>
+  </si>
+  <si>
+    <t>User should not be able to delete a moon by its ID</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to remove Planets from the Planetarium</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to remove Planets from the Planetarium, Negative Scenario</t>
+  </si>
+  <si>
+    <t>User should not be able to delete a planet by its ID</t>
+  </si>
+  <si>
+    <t>User wants to see all the available celestial bodies in planetarium</t>
+  </si>
+  <si>
+    <t>User should be able to see new added celestial bodies.</t>
+  </si>
+  <si>
+    <t>User should be not able to see newly deleted celestial bodies.</t>
   </si>
 </sst>
 </file>
@@ -302,15 +359,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECDEB107-C880-47DF-A16A-99B7E63DBCE4}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,7 +740,7 @@
     <col min="21" max="21" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
@@ -733,198 +799,255 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:21" s="7" customFormat="1" ht="101" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:21" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:21" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:21" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:21" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-    </row>
-    <row r="5" spans="1:21" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+    </row>
+    <row r="6" spans="1:21" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:21" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:21" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:21" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
+      <c r="G7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:21" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:21" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:21" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="1:21" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="1" t="s">
+      <c r="I9" s="4"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:21" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:21" ht="45.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:21" ht="45.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:21" ht="45.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:21" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:21" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:21" ht="54.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:21" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="3"/>
+      <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:21" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:21" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:21" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="1" t="s">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" ht="81.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="1" t="s">
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="1" t="s">
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" ht="63.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="1" t="s">
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H22" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>